<commit_message>
editPrj-done, allPrjs-done, chngPass-done, notyServ-added
</commit_message>
<xml_diff>
--- a/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acheb\Documents\Programming\SoftUni\softuni-courses\javascript-spa\March-2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo-PC\GitHub\currentProjects\IssueTrackingSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -150,17 +150,37 @@
   <si>
     <t>-&gt;Edit Project Page</t>
   </si>
+  <si>
+    <t>pepster</t>
+  </si>
+  <si>
+    <t>Plamena Nedelcheva Georgieva</t>
+  </si>
+  <si>
+    <t>https://github.com/plmng/IssueTrackingSystem</t>
+  </si>
+  <si>
+    <t>not set as buttons but links in navigations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,6 +212,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -288,12 +316,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,17 +334,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -324,35 +353,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,23 +477,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -496,23 +512,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -667,18 +666,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
@@ -692,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>13</v>
       </c>
@@ -700,23 +699,27 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
         <v>9</v>
       </c>
@@ -724,15 +727,17 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -742,7 +747,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
@@ -752,7 +757,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>27</v>
       </c>
@@ -760,7 +765,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -772,7 +777,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
@@ -782,7 +787,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
@@ -792,7 +797,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -802,7 +807,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
@@ -812,7 +817,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
@@ -822,7 +827,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
@@ -832,7 +837,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
@@ -842,7 +847,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -852,7 +857,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
@@ -862,7 +867,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
@@ -872,7 +877,7 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
@@ -882,17 +887,19 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4">
+        <v>10</v>
+      </c>
       <c r="D23" s="4">
         <v>10</v>
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
         <v>28</v>
       </c>
@@ -900,7 +907,7 @@
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
@@ -910,7 +917,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
@@ -920,7 +927,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
@@ -928,17 +935,21 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6">
+        <v>10</v>
+      </c>
       <c r="D28" s="6">
         <v>10</v>
       </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
         <v>32</v>
       </c>
@@ -948,7 +959,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>33</v>
       </c>
@@ -958,7 +969,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
         <v>34</v>
       </c>
@@ -968,13 +979,13 @@
       </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>
@@ -991,7 +1002,10 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add issue, add project via modal added
</commit_message>
<xml_diff>
--- a/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -160,7 +160,19 @@
     <t>https://github.com/plmng/IssueTrackingSystem</t>
   </si>
   <si>
-    <t>not set as buttons but links in navigations</t>
+    <t>done</t>
+  </si>
+  <si>
+    <t>evetualy todo: in case of error - to refresh so inputs to be empty</t>
+  </si>
+  <si>
+    <t>Add project button not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">links to project-view, issue-view </t>
+  </si>
+  <si>
+    <t>comments shown and add abiliti</t>
   </si>
 </sst>
 </file>
@@ -320,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -377,11 +389,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -666,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,11 +746,11 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -791,37 +806,51 @@
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
       <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
       <c r="D14" s="4">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4">
+        <v>10</v>
+      </c>
       <c r="D15" s="4">
         <v>10</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
@@ -831,7 +860,9 @@
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
       <c r="D17" s="4">
         <v>5</v>
       </c>
@@ -871,7 +902,9 @@
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4">
+        <v>10</v>
+      </c>
       <c r="D21" s="4">
         <v>10</v>
       </c>
@@ -881,7 +914,9 @@
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
       <c r="D22" s="4">
         <v>5</v>
       </c>
@@ -911,11 +946,15 @@
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6">
+        <v>20</v>
+      </c>
       <c r="D25" s="6">
         <v>20</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
@@ -946,7 +985,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -985,7 +1024,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>

<commit_message>
cleaning code, documentation edit
</commit_message>
<xml_diff>
--- a/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/Documentation/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -163,17 +163,14 @@
     <t>all is done</t>
   </si>
   <si>
-    <t>filter bug to fix!</t>
-  </si>
-  <si>
-    <t>note ! add issue for admin is removed because current page specification, I left only in admin’s all projects page!/</t>
+    <t>note ! ADD ISSUE for admin is removed because current page specification, I left only in admin’s all projects page!/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,23 +227,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF92D050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -347,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -410,14 +401,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -701,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,19 +791,21 @@
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4">
         <v>20</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4">
@@ -822,10 +814,12 @@
       <c r="D12" s="4">
         <v>30</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4">
@@ -839,11 +833,11 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
@@ -853,7 +847,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="4">
@@ -871,13 +865,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
-      <c r="E16" s="25" t="s">
-        <v>40</v>
+      <c r="E16" s="26" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1004,11 +998,15 @@
       <c r="B26" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6">
+        <v>20</v>
+      </c>
       <c r="D26" s="6">
         <v>20</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
@@ -1037,13 +1035,13 @@
         <v>31</v>
       </c>
       <c r="C29" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D29" s="6">
         <v>10</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>39</v>
+      <c r="E29" s="24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1064,7 +1062,9 @@
       <c r="B31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="6">
+        <v>5</v>
+      </c>
       <c r="D31" s="6">
         <v>5</v>
       </c>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>